<commit_message>
AZ2522021|2:37PM Adding Parameters for E-1
</commit_message>
<xml_diff>
--- a/src/test/resources/PartRiskTestData/ProdEnv_Parameters.xlsx
+++ b/src/test/resources/PartRiskTestData/ProdEnv_Parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IdeaProjects\Z2Data-Part-Risk-Production-Version\src\test\resources\PartRiskTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1E12B0B-C39B-4607-BDE6-CD7EBE734BBF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89426469-869B-4EED-AA84-1B2E6977E186}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="2940" windowWidth="15375" windowHeight="7875" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7695" yWindow="1470" windowWidth="15375" windowHeight="7875" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SimpleSearch" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>Variable</t>
   </si>
@@ -65,6 +65,42 @@
   </si>
   <si>
     <t>Value</t>
+  </si>
+  <si>
+    <t>https://parts.z2data.com/RiskManager/Forecast?BomId=119090</t>
+  </si>
+  <si>
+    <t>https://parts.z2data.com/RiskManager/Compliance?BomId=119090</t>
+  </si>
+  <si>
+    <t>https://parts.z2data.com/RiskManager/Mitigation?BomId=119090</t>
+  </si>
+  <si>
+    <t>https://parts.z2data.com/RiskManager/Report?BomId=119090</t>
+  </si>
+  <si>
+    <t>https://parts.z2data.com/RiskManager/Scrub?BomId=119090</t>
+  </si>
+  <si>
+    <t>https://parts.z2data.com/RiskManager?BomId=119090</t>
+  </si>
+  <si>
+    <t>Pom_Dashboard_URL</t>
+  </si>
+  <si>
+    <t>Scrub_Tab_URL</t>
+  </si>
+  <si>
+    <t>Reports__Tab_URL</t>
+  </si>
+  <si>
+    <t>Mitigation_Tab_URL</t>
+  </si>
+  <si>
+    <t>Compliance_Tab_URL</t>
+  </si>
+  <si>
+    <t>ForeCast_Tab_URL</t>
   </si>
 </sst>
 </file>
@@ -170,15 +206,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -187,10 +220,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -584,16 +617,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMJ9"/>
+  <dimension ref="A1:AMJ17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="66.140625" style="7" bestFit="1" customWidth="1"/>
     <col min="3" max="1007" width="8.5703125" style="1" customWidth="1"/>
     <col min="1008" max="1024" width="9.140625" style="1" customWidth="1"/>
     <col min="1025" max="16384" width="9.140625" style="2"/>
@@ -608,46 +641,101 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="6" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
+      <c r="B6" s="6"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
+      <c r="A7" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
+      <c r="A8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
+      <c r="A9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B13" s="6"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B14" s="6"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B15" s="6"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B16" s="6"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
AZ2522021|3:11PM Adding Parameters for All navigation Urls
</commit_message>
<xml_diff>
--- a/src/test/resources/PartRiskTestData/ProdEnv_Parameters.xlsx
+++ b/src/test/resources/PartRiskTestData/ProdEnv_Parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IdeaProjects\Z2Data-Part-Risk-Production-Version\src\test\resources\PartRiskTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89426469-869B-4EED-AA84-1B2E6977E186}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7425A20C-D0E1-4CFC-ABA9-48930B9E9AAE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7695" yWindow="1470" windowWidth="15375" windowHeight="7875" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2790" yWindow="1170" windowWidth="15375" windowHeight="7875" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SimpleSearch" sheetId="1" r:id="rId1"/>
@@ -91,9 +91,6 @@
     <t>Scrub_Tab_URL</t>
   </si>
   <si>
-    <t>Reports__Tab_URL</t>
-  </si>
-  <si>
     <t>Mitigation_Tab_URL</t>
   </si>
   <si>
@@ -101,6 +98,9 @@
   </si>
   <si>
     <t>ForeCast_Tab_URL</t>
+  </si>
+  <si>
+    <t>Reports_Tab_URL</t>
   </si>
 </sst>
 </file>
@@ -619,8 +619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMJ17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -676,7 +676,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>13</v>
@@ -684,7 +684,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>14</v>
@@ -692,7 +692,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>15</v>
@@ -700,7 +700,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>16</v>

</xml_diff>